<commit_message>
correct heating timeline; other small changes
</commit_message>
<xml_diff>
--- a/data/transducer_pos/position_LUT.xlsx
+++ b/data/transducer_pos/position_LUT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Documents\repos\PRESTUS_forked\data\transducer_pos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAD0F0B-0CDA-4CCB-8FBF-744861F9A084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC5EF93-47A6-4C84-AD6C-4F470C00FCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11475" yWindow="4845" windowWidth="14040" windowHeight="12900" xr2:uid="{4D69DF98-64CF-452E-BA5F-6007EC62E4E7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D69DF98-64CF-452E-BA5F-6007EC62E4E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -428,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA51C0A-6640-4C0C-B172-10C012B16ABF}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,6 +600,52 @@
         <v>153</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>98</v>
+      </c>
+      <c r="C9">
+        <v>138</v>
+      </c>
+      <c r="D9">
+        <v>147</v>
+      </c>
+      <c r="E9">
+        <v>127</v>
+      </c>
+      <c r="F9">
+        <v>138</v>
+      </c>
+      <c r="G9">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
config with 2 differently shaped transducers
</commit_message>
<xml_diff>
--- a/data/transducer_pos/position_LUT.xlsx
+++ b/data/transducer_pos/position_LUT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Documents\repos\PRESTUS_forked\data\transducer_pos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC5EF93-47A6-4C84-AD6C-4F470C00FCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E291E7DE-890D-407B-8823-9BB372999422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D69DF98-64CF-452E-BA5F-6007EC62E4E7}"/>
   </bookViews>
@@ -431,7 +431,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>